<commit_message>
Added Transform & Fetch code in testcases package and added excel sheet for the same.
</commit_message>
<xml_diff>
--- a/TestingFramework/TestData/Regression.xlsx
+++ b/TestingFramework/TestData/Regression.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="525" windowWidth="14805" windowHeight="7590" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="585" windowWidth="14805" windowHeight="7530" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Organisation" sheetId="12" r:id="rId1"/>
@@ -14,14 +14,15 @@
     <sheet name="MultipleProjectAndModule" sheetId="17" r:id="rId5"/>
     <sheet name="studiologin" sheetId="18" r:id="rId6"/>
     <sheet name="test" sheetId="19" r:id="rId7"/>
-    <sheet name="Sheet3" sheetId="21" r:id="rId8"/>
+    <sheet name="EditMultipleProject" sheetId="21" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="22" r:id="rId9"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="612">
   <si>
     <t>Yes</t>
   </si>
@@ -2197,6 +2198,246 @@
   </si>
   <si>
     <t>Save Customerr</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">KagamiProjectName1 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KagamiProjectNamEdited1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">KagamiProjectName2 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KagamiProjectNamEdited2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">KagamiProjectName3 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KagamiProjectNamEdited3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">KagamiProjectName4 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KagamiProjectNamEdited4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">KagamiProjectName5 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KagamiProjectNamEdited5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Module13 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: EditedModule1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SubModule11 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedSubModule1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Module33 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedModule3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Module42 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedModule4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SubModule22 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedSubModule2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SubModule33 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedSubModule3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SubModule41 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedSubModule4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SubModule53 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedSubModule5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Module51 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedModule5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Module21 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: EditedModule2</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -5010,8 +5251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -6290,7 +6531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -6652,12 +6893,246 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>597</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>602</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>603</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>598</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>611</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>606</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>599</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>604</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>607</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>600</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>605</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>608</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>601</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>610</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>609</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>598</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>611</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>606</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>599</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>604</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>607</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>600</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>605</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>608</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>601</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>610</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>609</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Multiple project and process suite
</commit_message>
<xml_diff>
--- a/TestingFramework/TestData/Regression.xlsx
+++ b/TestingFramework/TestData/Regression.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="585" windowWidth="14805" windowHeight="7530" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="705" windowWidth="14805" windowHeight="7410" firstSheet="4" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Organisation" sheetId="12" r:id="rId1"/>
@@ -16,13 +16,15 @@
     <sheet name="test" sheetId="19" r:id="rId7"/>
     <sheet name="EditMultipleProject" sheetId="21" r:id="rId8"/>
     <sheet name="Sheet1" sheetId="22" r:id="rId9"/>
+    <sheet name="Sheet2" sheetId="23" r:id="rId10"/>
+    <sheet name="ProcessAndPolicies" sheetId="24" r:id="rId11"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1709" uniqueCount="733">
   <si>
     <t>Yes</t>
   </si>
@@ -2438,6 +2440,1406 @@
       </rPr>
       <t>: EditedModule2</t>
     </r>
+  </si>
+  <si>
+    <t>TestCase id</t>
+  </si>
+  <si>
+    <t>TC_01</t>
+  </si>
+  <si>
+    <t>TC_02</t>
+  </si>
+  <si>
+    <t>super</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">KagamiProjectName6 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KagamiProjectNamEdited6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">KagamiProjectName7 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KagamiProjectNamEdited7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">KagamiProjectName8 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KagamiProjectNamEdited8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">KagamiProjectName9 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KagamiProjectNamEdited9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">KagamiProjectName10 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KagamiProjectNamEdited10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">KagamiProjectName11 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KagamiProjectNamEdited11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">KagamiProjectName12 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KagamiProjectNamEdited12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">KagamiProjectName13 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KagamiProjectNamEdited13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">KagamiProjectName14 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KagamiProjectNamEdited14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">KagamiProjectName15 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KagamiProjectNamEdited15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">KagamiProjectName16 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KagamiProjectNamEdited16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">KagamiProjectName17 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KagamiProjectNamEdited17</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">KagamiProjectName18 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KagamiProjectNamEdited18</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">KagamiProjectName19 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KagamiProjectNamEdited19</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">KagamiProjectName20 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KagamiProjectNamEdited20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Module62 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedModule6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SubModule62 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedSubModule6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Module71 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedModule7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SubModule73 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedSubModule7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>Module71, Module72,Module75</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Module83 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedModule8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SubModule82 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedSubModule8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Module91 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedModule9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>SubModule92, SubModule93, SubModule94</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SubModule93 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedSubModule9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Module102 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedModule10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Module112 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedModule11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SubModule103 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedSubModule10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SubModule112 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedSubModule11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Module122 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedModule12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SubModule122 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedSubModule12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Module133 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedModule13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SubModule133 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedSubModule13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Module141 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedModule14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SubModule143 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedSubModule14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Module151 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedModule15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SubModule152 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedSubModule15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>Module161, Module162,Module163</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Module162 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedModule16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>SubModule161, SubModule162, SubModule163</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SubModule163 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedSubModule16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>Module171, Module172,Module173</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Module173 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedModule17</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>SubModule171, SubModule172, SubModule173</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SubModule173 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedSubModule17</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>Module181, Module182,Module183</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Module181 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedModule18</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>SubModule181, SubModule182, SubModule183</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SubModule182 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedSubModule18</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>Module191, Module192,Module193</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Module193 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedModule19</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>SubModule191, SubModule192, SubModule193</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SubModule191 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedSubModule19</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>Module201, Module202,Module203</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Module201 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedModule20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>SubModule201, SubModule202, SubModule203</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SubModule202 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EditedSubModule20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>Process11 Process41 Prcess61</t>
+  </si>
+  <si>
+    <t>Process12 Process42 Prcess62</t>
+  </si>
+  <si>
+    <t>Process13 Process43 Prcess63</t>
+  </si>
+  <si>
+    <t>Process14 Process44 Prcess64</t>
+  </si>
+  <si>
+    <t>Process15 Process45 Prcess65</t>
+  </si>
+  <si>
+    <t>Process15 Process45 Prcess66</t>
+  </si>
+  <si>
+    <t>Process15 Process45 Prcess67</t>
+  </si>
+  <si>
+    <t>Process15 Process45 Prcess68</t>
+  </si>
+  <si>
+    <t>Process15 Process45 Prcess69</t>
+  </si>
+  <si>
+    <t>Process15 Process45 Prcess70</t>
+  </si>
+  <si>
+    <t>Process15 Process45 Prcess71</t>
+  </si>
+  <si>
+    <t>Process15 Process45 Prcess72</t>
+  </si>
+  <si>
+    <t>Process15 Process45 Prcess73</t>
+  </si>
+  <si>
+    <t>Process15 Process45 Prcess74</t>
+  </si>
+  <si>
+    <t>Process15 Process45 Prcess75</t>
+  </si>
+  <si>
+    <t>Process15 Process45 Prcess76</t>
+  </si>
+  <si>
+    <t>Process15 Process45 Prcess77</t>
+  </si>
+  <si>
+    <t>Process15 Process45 Prcess78</t>
+  </si>
+  <si>
+    <t>Process15 Process45 Prcess79</t>
+  </si>
+  <si>
+    <t>Process15 Process45 Prcess80</t>
+  </si>
+  <si>
+    <t>TC_ID</t>
+  </si>
+  <si>
+    <t>TC_03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AutomationTestProjectTest </t>
+  </si>
+  <si>
+    <t>TC_04</t>
+  </si>
+  <si>
+    <t>Entity Attributes</t>
+  </si>
+  <si>
+    <t>Select Rules</t>
+  </si>
+  <si>
+    <t>Policies</t>
+  </si>
+  <si>
+    <t>Restrictions</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>Business Validation</t>
+  </si>
+  <si>
+    <t>TC_05</t>
+  </si>
+  <si>
+    <t>LeaveProcess</t>
+  </si>
+  <si>
+    <t>EmployeeDetails</t>
+  </si>
+  <si>
+    <t>employeeName</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>TC_06</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>TC_07</t>
+  </si>
+  <si>
+    <t>Edit</t>
+  </si>
+  <si>
+    <t>pcEmbedEdit</t>
+  </si>
+  <si>
+    <t>pcModalEdit</t>
+  </si>
+  <si>
+    <t>TC_08</t>
+  </si>
+  <si>
+    <t>TC_09</t>
+  </si>
+  <si>
+    <t>TC_10</t>
+  </si>
+  <si>
+    <t>TC_11</t>
+  </si>
+  <si>
+    <t>TC_12</t>
+  </si>
+  <si>
+    <t>TC_13</t>
+  </si>
+  <si>
+    <t>TC_14</t>
+  </si>
+  <si>
+    <t>TC_15</t>
+  </si>
+  <si>
+    <t>TC_16</t>
+  </si>
+  <si>
+    <t>TC_17</t>
+  </si>
+  <si>
+    <t>TC_18</t>
+  </si>
+  <si>
+    <t>TC_19</t>
+  </si>
+  <si>
+    <t>TC_20</t>
+  </si>
+  <si>
+    <t>TC_21</t>
+  </si>
+  <si>
+    <t>pcMultiEdit</t>
+  </si>
+  <si>
+    <t>edit</t>
+  </si>
+  <si>
+    <t>editTabbed</t>
+  </si>
+  <si>
+    <t>EmployeeDetails.employeeName,not equals,Edit1111 and
+EmployeeDetails.employeeName,not equals,Edit1212</t>
+  </si>
+  <si>
+    <t>EmployeeDetails.employeeName,not equals,Edit211 and
+EmployeeDetails.employeeName,not equals,Edit221</t>
   </si>
 </sst>
 </file>
@@ -2539,7 +3941,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2562,12 +3964,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2586,6 +4001,10 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2953,6 +4372,1852 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>462</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>492</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>522</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>463</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>523</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>464</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>524</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>495</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>525</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>466</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>496</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>526</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>497</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>527</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>468</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>498</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>528</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>469</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>499</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>529</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>500</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>530</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>501</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>531</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>442</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>502</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>532</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>503</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>533</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
+        <v>415</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>504</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>534</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>475</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>505</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>535</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>446</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>476</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>506</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>536</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>447</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>477</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>507</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>537</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>419</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>448</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>508</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>538</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>449</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>479</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>509</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>539</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>421</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>480</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>510</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>540</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>422</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>511</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>541</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>423</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>452</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>512</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>542</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>513</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>543</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>454</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>484</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>544</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>455</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>485</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>545</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>486</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>546</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>457</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>517</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>547</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>488</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>518</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>548</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>489</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>519</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>549</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>460</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>490</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>520</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>550</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>521</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>551</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>581</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="55.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="56" style="2" customWidth="1"/>
+    <col min="11" max="11" width="38.140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="56" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>693</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>697</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>698</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>705</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>707</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>731</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="17" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>705</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>709</v>
+      </c>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+    </row>
+    <row r="6" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>705</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>707</v>
+      </c>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+    </row>
+    <row r="7" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>705</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>709</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+    </row>
+    <row r="8" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>705</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>707</v>
+      </c>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+    </row>
+    <row r="9" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>705</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>709</v>
+      </c>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+    </row>
+    <row r="10" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>705</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>707</v>
+      </c>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+    </row>
+    <row r="11" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>705</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>709</v>
+      </c>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+    </row>
+    <row r="12" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>705</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>709</v>
+      </c>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+    </row>
+    <row r="13" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>705</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>709</v>
+      </c>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+    </row>
+    <row r="14" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>705</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>709</v>
+      </c>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+    </row>
+    <row r="15" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>705</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>707</v>
+      </c>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+    </row>
+    <row r="16" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>705</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>709</v>
+      </c>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+    </row>
+    <row r="17" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>705</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>709</v>
+      </c>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+    </row>
+    <row r="18" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>705</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>709</v>
+      </c>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+    </row>
+    <row r="19" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>705</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>707</v>
+      </c>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+    </row>
+    <row r="20" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
@@ -5251,8 +8516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -6494,32 +9759,50 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>612</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>233</v>
+        <v>613</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>233</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>615</v>
       </c>
     </row>
   </sheetData>
@@ -6893,23 +10176,23 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>64</v>
       </c>
@@ -6929,7 +10212,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>597</v>
       </c>
@@ -6946,10 +10229,11 @@
         <v>603</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>673</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>598</v>
       </c>
@@ -6966,10 +10250,11 @@
         <v>606</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>674</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>599</v>
       </c>
@@ -6986,10 +10271,11 @@
         <v>607</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>675</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>600</v>
       </c>
@@ -7006,10 +10292,11 @@
         <v>608</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>676</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>601</v>
       </c>
@@ -7026,8 +10313,354 @@
         <v>609</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>220</v>
-      </c>
+        <v>677</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>616</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>631</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>632</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>678</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>617</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>635</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>633</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>634</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>679</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>618</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>636</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>637</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>680</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>619</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>638</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>639</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>640</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>681</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>620</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>641</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>682</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>621</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>644</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>683</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>622</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>646</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>684</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>623</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>647</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>648</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>685</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>624</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>649</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>650</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>686</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>625</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>651</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>652</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>687</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>626</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>653</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>654</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>655</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>656</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>688</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>627</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>657</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>658</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>659</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>660</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>689</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>628</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>661</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>662</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>663</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>664</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>690</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>629</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>665</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>666</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>667</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>691</v>
+      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>630</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>669</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>670</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>671</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>672</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>692</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>